<commit_message>
alterado processo e criado diretorios para alocar templates de artefatos
</commit_message>
<xml_diff>
--- a/data/processo.xlsx
+++ b/data/processo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrelerario/Desktop/delme/vue/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrelerario/Desktop/pros/proshow/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EE2D23-D73B-B04F-BF32-442A37BE6303}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8869CA08-513B-7D43-8888-9ACDF0F752BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="460" windowWidth="28040" windowHeight="17560" activeTab="4" xr2:uid="{5FF78378-EBA3-0B44-8062-CCA0B545436E}"/>
+    <workbookView xWindow="6980" yWindow="1900" windowWidth="28040" windowHeight="17560" xr2:uid="{5FF78378-EBA3-0B44-8062-CCA0B545436E}"/>
   </bookViews>
   <sheets>
     <sheet name="visaoestatica" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>Papel op</t>
   </si>
   <si>
-    <t>link:modelo.docx</t>
-  </si>
-  <si>
     <t>Atividade referente a eleicitação de requisitos. Nesta o analista entrevista o cliente com o propósito de montar um documento de requisitos</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>Lista contendo os requisitos e o contrato com o cliente</t>
   </si>
   <si>
-    <t>link:contrato.docx</t>
-  </si>
-  <si>
     <t>ID Entrada</t>
   </si>
   <si>
@@ -157,25 +151,31 @@
     <t>link:Guia</t>
   </si>
   <si>
-    <t>padrao.pdf</t>
-  </si>
-  <si>
     <t>Notação UML</t>
   </si>
   <si>
-    <t>uml.pdf</t>
-  </si>
-  <si>
     <t>Manual como entrevistar</t>
   </si>
   <si>
-    <t>entrevista.pdf</t>
-  </si>
-  <si>
     <t>Responsavel pela interação com cliente. Definição de requisitos</t>
   </si>
   <si>
     <t>Desenvolver todo o código do produto</t>
+  </si>
+  <si>
+    <t>artefatos\modelo.docx</t>
+  </si>
+  <si>
+    <t>artefatos\contrato.docx</t>
+  </si>
+  <si>
+    <t>guidance\entrevista.pdf</t>
+  </si>
+  <si>
+    <t>guidance\padrao.pdf</t>
+  </si>
+  <si>
+    <t>guidance\uml.pdf</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E29CB1A-062A-EC4A-8D02-E29BA1CBBF57}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1561,28 +1561,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>12</v>
@@ -1597,16 +1597,16 @@
         <v>16</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -1617,7 +1617,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="8" t="str">
         <f>IFERROR(VLOOKUP(D2,artefatos!$A$1:$D$40,2,),"")</f>
@@ -1669,7 +1669,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="8">
         <v>1</v>
@@ -1721,7 +1721,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="8">
         <v>2</v>
@@ -1779,7 +1779,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="8">
         <v>2</v>
@@ -2331,7 +2331,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2342,7 +2342,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2361,7 +2361,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="73.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2375,7 +2375,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2383,13 +2383,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2397,13 +2397,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2411,10 +2411,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2427,26 +2427,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF52C8F-96A4-644E-8B3C-1A3EAEF42320}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>39</v>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2454,7 +2454,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -2465,10 +2465,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2476,10 +2476,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustado nome dos arquivos
</commit_message>
<xml_diff>
--- a/data/processo.xlsx
+++ b/data/processo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrelerario/Desktop/pros/proshow/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8869CA08-513B-7D43-8888-9ACDF0F752BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768D4EE7-ECFA-DC40-8153-EAC5F0060C90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6980" yWindow="1900" windowWidth="28040" windowHeight="17560" xr2:uid="{5FF78378-EBA3-0B44-8062-CCA0B545436E}"/>
   </bookViews>
@@ -163,19 +163,19 @@
     <t>Desenvolver todo o código do produto</t>
   </si>
   <si>
-    <t>artefatos\modelo.docx</t>
-  </si>
-  <si>
     <t>artefatos\contrato.docx</t>
   </si>
   <si>
     <t>guidance\entrevista.pdf</t>
   </si>
   <si>
-    <t>guidance\padrao.pdf</t>
-  </si>
-  <si>
     <t>guidance\uml.pdf</t>
+  </si>
+  <si>
+    <t>artefatos\ListaRequisitos.docx</t>
+  </si>
+  <si>
+    <t>guidance\convencions.pdf</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2355,13 +2355,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="73.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2389,7 +2389,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2403,7 +2403,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2428,14 +2428,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2457,7 +2457,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2468,7 +2468,7 @@
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2479,7 +2479,7 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste na exibição dos dados
</commit_message>
<xml_diff>
--- a/data/processo.xlsx
+++ b/data/processo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrelerario/Desktop/pros/proshow/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37FF415-58B8-1C4D-BA82-47BD47E12C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D36F423-7D6B-CF47-AC23-6BA44445D90B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="1900" windowWidth="28040" windowHeight="17560" xr2:uid="{5FF78378-EBA3-0B44-8062-CCA0B545436E}"/>
+    <workbookView xWindow="6980" yWindow="1900" windowWidth="28040" windowHeight="17560" activeTab="1" xr2:uid="{5FF78378-EBA3-0B44-8062-CCA0B545436E}"/>
   </bookViews>
   <sheets>
     <sheet name="visaoestatica" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>guidance\convencions.pdf</t>
+  </si>
+  <si>
+    <t>fim</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E29CB1A-062A-EC4A-8D02-E29BA1CBBF57}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -1528,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5859C381-D0C5-5C41-95FA-D7C9ED4B577D}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1836,7 +1839,12 @@
       </c>
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="C6" s="9"/>
       <c r="E6" s="8" t="str">
         <f>IFERROR(VLOOKUP(D6,artefatos!$A$1:$D$40,2,),"")</f>

</xml_diff>

<commit_message>
Ajuste para exibição das tabelas quando o campo Nome==undefined
</commit_message>
<xml_diff>
--- a/data/processo.xlsx
+++ b/data/processo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrelerario/Desktop/pros/proshow/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D36F423-7D6B-CF47-AC23-6BA44445D90B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A20F67E-59CB-4146-8ABF-ECC120037B1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6980" yWindow="1900" windowWidth="28040" windowHeight="17560" activeTab="1" xr2:uid="{5FF78378-EBA3-0B44-8062-CCA0B545436E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>guidance\convencions.pdf</t>
-  </si>
-  <si>
-    <t>fim</t>
   </si>
 </sst>
 </file>
@@ -615,31 +612,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$F$49,2,),"")</f>
         <v>Elicitar</v>
       </c>
       <c r="C2" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D2" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E2" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$49,9,),"")</f>
         <v>Requisitos</v>
       </c>
       <c r="F2" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G2" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$49,13,),"")</f>
         <v>Analista</v>
       </c>
       <c r="H2" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A2,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
@@ -648,31 +645,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$F$49,2,),"")</f>
         <v>Especificar</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$50,5,)," ")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$49,5,)," ")</f>
         <v>Requisitos</v>
       </c>
       <c r="D3" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E3" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$49,9,),"")</f>
         <v>Contrato</v>
       </c>
       <c r="F3" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G3" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$49,13,),"")</f>
         <v>Analista</v>
       </c>
       <c r="H3" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A3,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
@@ -681,31 +678,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$F$49,2,),"")</f>
         <v>Validar</v>
       </c>
       <c r="C4" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$49,5,),"")</f>
         <v>Contrato</v>
       </c>
       <c r="D4" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E4" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$49,9,),"")</f>
         <v>Contrato</v>
       </c>
       <c r="F4" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$49,11,),"")</f>
         <v>Requisitos</v>
       </c>
       <c r="G4" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$49,13,),"")</f>
         <v>Analista</v>
       </c>
       <c r="H4" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A4,atividades!$A$1:$O$49,15,),"")</f>
         <v>Codificador</v>
       </c>
     </row>
@@ -714,811 +711,811 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$F$49,2,),"")</f>
         <v>Desenvolver</v>
       </c>
       <c r="C5" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$49,5,),"")</f>
         <v>Contrato</v>
       </c>
       <c r="D5" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$49,7,),"")</f>
         <v>Requisitos</v>
       </c>
       <c r="E5" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$49,9,),"")</f>
         <v>Código fonte</v>
       </c>
       <c r="F5" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$50,11,),"")</f>
-        <v/>
+        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$49,11,),"")</f>
+        <v>Requisitos</v>
       </c>
       <c r="G5" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$50,13,),"")</f>
-        <v>Codificador</v>
+        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$49,13,),"")</f>
+        <v>Analista</v>
       </c>
       <c r="H5" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A5,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C6" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D6" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E6" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F6" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G6" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H6" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A6,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C7" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D7" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E7" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F7" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G7" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H7" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A7,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C8" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D8" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E8" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F8" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G8" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H8" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A8,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C9" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D9" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E9" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F9" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G9" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H9" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A9,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C10" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D10" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E10" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F10" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G10" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H10" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A10,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C11" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D11" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E11" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F11" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G11" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H11" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A11,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C12" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D12" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E12" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F12" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G12" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H12" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A12,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C13" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D13" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E13" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F13" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G13" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H13" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A13,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C14" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D14" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E14" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F14" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G14" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H14" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A14,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C15" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D15" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E15" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F15" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G15" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H15" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A15,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C16" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D16" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E16" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F16" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G16" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H16" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A16,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C17" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D17" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E17" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F17" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G17" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H17" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A17,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C18" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D18" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E18" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F18" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G18" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H18" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A18,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C19" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D19" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E19" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F19" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G19" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H19" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A19,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C20" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D20" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E20" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F20" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G20" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H20" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A20,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C21" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D21" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E21" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F21" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G21" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H21" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A21,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C22" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D22" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E22" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F22" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G22" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H22" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A22,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C23" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D23" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E23" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F23" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G23" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H23" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A23,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C24" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D24" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E24" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F24" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G24" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H24" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A24,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C25" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D25" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E25" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F25" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G25" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H25" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A25,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C26" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D26" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E26" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F26" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G26" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H26" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A26,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C27" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D27" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E27" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F27" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G27" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H27" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A27,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C28" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D28" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E28" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F28" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G28" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H28" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A28,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
       <c r="C29" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$50,5,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$49,5,),"")</f>
         <v/>
       </c>
       <c r="D29" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$50,7,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$49,7,),"")</f>
         <v/>
       </c>
       <c r="E29" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$50,9,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$49,9,),"")</f>
         <v/>
       </c>
       <c r="F29" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$50,11,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$49,11,),"")</f>
         <v/>
       </c>
       <c r="G29" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$50,13,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$49,13,),"")</f>
         <v/>
       </c>
       <c r="H29" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$50,15,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A29,atividades!$A$1:$O$49,15,),"")</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A30,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A30,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A31,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A31,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A32,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A32,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A33,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A33,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A34,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A34,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A35,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A35,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A36,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A36,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A37,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A37,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A38,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A38,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="str">
-        <f>IFERROR(VLOOKUP(visaoestatica!A39,atividades!$A$1:$F$50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(visaoestatica!A39,atividades!$A$1:$F$49,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -1529,10 +1526,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5859C381-D0C5-5C41-95FA-D7C9ED4B577D}">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1806,18 +1803,18 @@
         <v>Código fonte</v>
       </c>
       <c r="J5" s="8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K5" s="8" t="str">
         <f>IFERROR(VLOOKUP(J5,artefatos!$A$1:$D$40,2,),"")</f>
-        <v/>
+        <v>Requisitos</v>
       </c>
       <c r="L5" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5" s="8" t="str">
         <f>IFERROR(VLOOKUP(L5,papeis!$A$1:$C$38,2,),"")</f>
-        <v>Codificador</v>
+        <v>Analista</v>
       </c>
       <c r="O5" s="8" t="str">
         <f>IFERROR(VLOOKUP(N5,papeis!$A$1:$C$38,2,),"")</f>
@@ -1839,12 +1836,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="A6" s="7"/>
       <c r="C6" s="9"/>
       <c r="E6" s="8" t="str">
         <f>IFERROR(VLOOKUP(D6,artefatos!$A$1:$D$40,2,),"")</f>
@@ -1930,28 +1922,12 @@
     <row r="9" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="C9" s="9"/>
-      <c r="E9" s="8" t="str">
-        <f>IFERROR(VLOOKUP(D9,artefatos!$A$1:$D$40,2,),"")</f>
-        <v/>
-      </c>
-      <c r="G9" s="8" t="str">
-        <f>IFERROR(VLOOKUP(F9,artefatos!$A$1:$D$40,2,),"")</f>
-        <v/>
-      </c>
-      <c r="I9" s="8" t="str">
-        <f>IFERROR(VLOOKUP(H9,artefatos!$A$1:$D$40,2,),"")</f>
-        <v/>
-      </c>
-      <c r="K9" s="8" t="str">
-        <f>IFERROR(VLOOKUP(J9,artefatos!$A$1:$D$40,2,),"")</f>
-        <v/>
-      </c>
       <c r="M9" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L9,papeis!$A$1:$C$38,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L9,papeis!A9:C46,2,),"")</f>
         <v/>
       </c>
       <c r="O9" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N9,papeis!$A$1:$C$38,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N9,papeis!A9:C46,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -1959,11 +1935,11 @@
       <c r="A10" s="7"/>
       <c r="C10" s="9"/>
       <c r="M10" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L10,papeis!A9:C46,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L10,papeis!A10:C47,2,),"")</f>
         <v/>
       </c>
       <c r="O10" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N10,papeis!A9:C46,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N10,papeis!A10:C47,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -1971,11 +1947,11 @@
       <c r="A11" s="7"/>
       <c r="C11" s="9"/>
       <c r="M11" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L11,papeis!A10:C47,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L11,papeis!A11:C48,2,),"")</f>
         <v/>
       </c>
       <c r="O11" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N11,papeis!A10:C47,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N11,papeis!A11:C48,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -1983,11 +1959,11 @@
       <c r="A12" s="7"/>
       <c r="C12" s="9"/>
       <c r="M12" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L12,papeis!A11:C48,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L12,papeis!A12:C49,2,),"")</f>
         <v/>
       </c>
       <c r="O12" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N12,papeis!A11:C48,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N12,papeis!A12:C49,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -1995,11 +1971,11 @@
       <c r="A13" s="7"/>
       <c r="C13" s="9"/>
       <c r="M13" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L13,papeis!A12:C49,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L13,papeis!A13:C50,2,),"")</f>
         <v/>
       </c>
       <c r="O13" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N13,papeis!A12:C49,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N13,papeis!A13:C50,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2007,11 +1983,11 @@
       <c r="A14" s="7"/>
       <c r="C14" s="9"/>
       <c r="M14" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L14,papeis!A13:C50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L14,papeis!A14:C51,2,),"")</f>
         <v/>
       </c>
       <c r="O14" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N14,papeis!A13:C50,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N14,papeis!A14:C51,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2019,11 +1995,11 @@
       <c r="A15" s="7"/>
       <c r="C15" s="9"/>
       <c r="M15" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L15,papeis!A14:C51,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L15,papeis!A15:C52,2,),"")</f>
         <v/>
       </c>
       <c r="O15" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N15,papeis!A14:C51,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N15,papeis!A15:C52,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2031,11 +2007,11 @@
       <c r="A16" s="7"/>
       <c r="C16" s="9"/>
       <c r="M16" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L16,papeis!A15:C52,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L16,papeis!A16:C53,2,),"")</f>
         <v/>
       </c>
       <c r="O16" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N16,papeis!A15:C52,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N16,papeis!A16:C53,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2043,11 +2019,11 @@
       <c r="A17" s="7"/>
       <c r="C17" s="9"/>
       <c r="M17" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L17,papeis!A16:C53,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L17,papeis!A17:C54,2,),"")</f>
         <v/>
       </c>
       <c r="O17" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N17,papeis!A16:C53,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N17,papeis!A17:C54,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2055,11 +2031,11 @@
       <c r="A18" s="7"/>
       <c r="C18" s="9"/>
       <c r="M18" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L18,papeis!A17:C54,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L18,papeis!A18:C55,2,),"")</f>
         <v/>
       </c>
       <c r="O18" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N18,papeis!A17:C54,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N18,papeis!A18:C55,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2067,11 +2043,11 @@
       <c r="A19" s="7"/>
       <c r="C19" s="9"/>
       <c r="M19" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L19,papeis!A18:C55,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L19,papeis!A19:C56,2,),"")</f>
         <v/>
       </c>
       <c r="O19" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N19,papeis!A18:C55,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N19,papeis!A19:C56,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2079,11 +2055,11 @@
       <c r="A20" s="7"/>
       <c r="C20" s="9"/>
       <c r="M20" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L20,papeis!A19:C56,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L20,papeis!A20:C57,2,),"")</f>
         <v/>
       </c>
       <c r="O20" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N20,papeis!A19:C56,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N20,papeis!A20:C57,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2091,11 +2067,11 @@
       <c r="A21" s="7"/>
       <c r="C21" s="9"/>
       <c r="M21" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L21,papeis!A20:C57,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L21,papeis!A21:C58,2,),"")</f>
         <v/>
       </c>
       <c r="O21" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N21,papeis!A20:C57,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N21,papeis!A21:C58,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2103,11 +2079,11 @@
       <c r="A22" s="7"/>
       <c r="C22" s="9"/>
       <c r="M22" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L22,papeis!A21:C58,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L22,papeis!A22:C59,2,),"")</f>
         <v/>
       </c>
       <c r="O22" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N22,papeis!A21:C58,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N22,papeis!A22:C59,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2115,11 +2091,11 @@
       <c r="A23" s="7"/>
       <c r="C23" s="9"/>
       <c r="M23" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L23,papeis!A22:C59,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L23,papeis!A23:C60,2,),"")</f>
         <v/>
       </c>
       <c r="O23" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N23,papeis!A22:C59,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N23,papeis!A23:C60,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2127,11 +2103,11 @@
       <c r="A24" s="7"/>
       <c r="C24" s="9"/>
       <c r="M24" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L24,papeis!A23:C60,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L24,papeis!A24:C61,2,),"")</f>
         <v/>
       </c>
       <c r="O24" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N24,papeis!A23:C60,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N24,papeis!A24:C61,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2139,11 +2115,11 @@
       <c r="A25" s="7"/>
       <c r="C25" s="9"/>
       <c r="M25" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L25,papeis!A24:C61,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L25,papeis!A25:C62,2,),"")</f>
         <v/>
       </c>
       <c r="O25" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N25,papeis!A24:C61,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N25,papeis!A25:C62,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2151,11 +2127,11 @@
       <c r="A26" s="7"/>
       <c r="C26" s="9"/>
       <c r="M26" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L26,papeis!A25:C62,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L26,papeis!A26:C63,2,),"")</f>
         <v/>
       </c>
       <c r="O26" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N26,papeis!A25:C62,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N26,papeis!A26:C63,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2163,11 +2139,11 @@
       <c r="A27" s="7"/>
       <c r="C27" s="9"/>
       <c r="M27" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L27,papeis!A26:C63,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L27,papeis!A27:C64,2,),"")</f>
         <v/>
       </c>
       <c r="O27" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N27,papeis!A26:C63,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N27,papeis!A27:C64,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2175,11 +2151,11 @@
       <c r="A28" s="7"/>
       <c r="C28" s="9"/>
       <c r="M28" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L28,papeis!A27:C64,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L28,papeis!A28:C65,2,),"")</f>
         <v/>
       </c>
       <c r="O28" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N28,papeis!A27:C64,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N28,papeis!A28:C65,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2187,11 +2163,11 @@
       <c r="A29" s="7"/>
       <c r="C29" s="9"/>
       <c r="M29" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L29,papeis!A28:C65,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L29,papeis!A29:C66,2,),"")</f>
         <v/>
       </c>
       <c r="O29" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N29,papeis!A28:C65,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N29,papeis!A29:C66,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2199,11 +2175,11 @@
       <c r="A30" s="7"/>
       <c r="C30" s="9"/>
       <c r="M30" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L30,papeis!A29:C66,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L30,papeis!A30:C67,2,),"")</f>
         <v/>
       </c>
       <c r="O30" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N30,papeis!A29:C66,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N30,papeis!A30:C67,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2211,11 +2187,11 @@
       <c r="A31" s="7"/>
       <c r="C31" s="9"/>
       <c r="M31" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L31,papeis!A30:C67,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L31,papeis!A31:C68,2,),"")</f>
         <v/>
       </c>
       <c r="O31" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N31,papeis!A30:C67,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N31,papeis!A31:C68,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2223,11 +2199,11 @@
       <c r="A32" s="7"/>
       <c r="C32" s="9"/>
       <c r="M32" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L32,papeis!A31:C68,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L32,papeis!A32:C69,2,),"")</f>
         <v/>
       </c>
       <c r="O32" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N32,papeis!A31:C68,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N32,papeis!A32:C69,2,),"")</f>
         <v/>
       </c>
     </row>
@@ -2235,73 +2211,61 @@
       <c r="A33" s="7"/>
       <c r="C33" s="9"/>
       <c r="M33" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L33,papeis!A32:C69,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L33,papeis!A33:C70,2,),"")</f>
         <v/>
       </c>
       <c r="O33" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N33,papeis!A32:C69,2,),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
-      <c r="C34" s="9"/>
-      <c r="M34" s="8" t="str">
-        <f>IFERROR(VLOOKUP(L34,papeis!A33:C70,2,),"")</f>
-        <v/>
-      </c>
-      <c r="O34" s="8" t="str">
-        <f>IFERROR(VLOOKUP(N34,papeis!A33:C70,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N33,papeis!A33:C70,2,),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M34" t="str">
+        <f>IFERROR(VLOOKUP(L34,papeis!A34:C71,2,),"")</f>
+        <v/>
+      </c>
+      <c r="O34" t="str">
+        <f>IFERROR(VLOOKUP(N34,papeis!A34:C71,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M35" t="str">
-        <f>IFERROR(VLOOKUP(L35,papeis!A34:C71,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L35,papeis!A35:C72,2,),"")</f>
         <v/>
       </c>
       <c r="O35" t="str">
-        <f>IFERROR(VLOOKUP(N35,papeis!A34:C71,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N35,papeis!A35:C72,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M36" t="str">
-        <f>IFERROR(VLOOKUP(L36,papeis!A35:C72,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L36,papeis!A36:C73,2,),"")</f>
         <v/>
       </c>
       <c r="O36" t="str">
-        <f>IFERROR(VLOOKUP(N36,papeis!A35:C72,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N36,papeis!A36:C73,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M37" t="str">
-        <f>IFERROR(VLOOKUP(L37,papeis!A36:C73,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L37,papeis!A37:C74,2,),"")</f>
         <v/>
       </c>
       <c r="O37" t="str">
-        <f>IFERROR(VLOOKUP(N37,papeis!A36:C73,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N37,papeis!A37:C74,2,),"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M38" t="str">
-        <f>IFERROR(VLOOKUP(L38,papeis!A37:C74,2,),"")</f>
+        <f>IFERROR(VLOOKUP(L38,papeis!A38:C75,2,),"")</f>
         <v/>
       </c>
       <c r="O38" t="str">
-        <f>IFERROR(VLOOKUP(N38,papeis!A37:C74,2,),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M39" t="str">
-        <f>IFERROR(VLOOKUP(L39,papeis!A38:C75,2,),"")</f>
-        <v/>
-      </c>
-      <c r="O39" t="str">
-        <f>IFERROR(VLOOKUP(N39,papeis!A38:C75,2,),"")</f>
+        <f>IFERROR(VLOOKUP(N38,papeis!A38:C75,2,),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>